<commit_message>
Add - se agregan los NMSE de la icwt mediante magnitude coefficients
</commit_message>
<xml_diff>
--- a/Configuración de banco de filtros y comparación del error NMSE.xlsx
+++ b/Configuración de banco de filtros y comparación del error NMSE.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976A6BC1-AA3F-452E-9805-BD8ADA931DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B172B3F-00EB-4A4B-97AA-FED6E03ED82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{546CBC35-C41A-4C5F-9A5B-D35005C1BB7E}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{546CBC35-C41A-4C5F-9A5B-D35005C1BB7E}"/>
   </bookViews>
   <sheets>
-    <sheet name="análisis" sheetId="1" r:id="rId1"/>
+    <sheet name="Error - banco de filtros" sheetId="1" r:id="rId1"/>
+    <sheet name="Error - magnitud coeficientes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t>G2_001.csv</t>
   </si>
@@ -280,6 +281,9 @@
   </si>
   <si>
     <t>bump</t>
+  </si>
+  <si>
+    <t>Análisis: Error calculado en base a la magnitud de los coeficientes reales ()</t>
   </si>
 </sst>
 </file>
@@ -328,7 +332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +378,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFABC5AC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,66 +459,87 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -501,9 +550,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFABC5AC"/>
       <color rgb="FFC2FCB2"/>
       <color rgb="FFC1F1C1"/>
-      <color rgb="FFABC5AC"/>
       <color rgb="FF5D8F41"/>
       <color rgb="FF99CC00"/>
     </mruColors>
@@ -836,313 +885,316 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714202BB-DA4E-4E71-9EB2-9A84168B02F8}">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="B3:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="14" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="7" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="14" t="s">
+      <c r="D27" s="16"/>
+      <c r="E27" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="14" t="s">
+      <c r="F27" s="16"/>
+      <c r="G27" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="16" t="s">
+      <c r="H27" s="16"/>
+      <c r="I27" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="4">
+      <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5">
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11">
         <v>3</v>
       </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="6">
+      <c r="H28" s="11"/>
+      <c r="I28" s="3">
         <v>1.1674E-30</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="9">
+      <c r="B29" s="4">
         <v>2</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="11">
+      <c r="D29" s="12"/>
+      <c r="E29" s="13">
         <v>10</v>
       </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="11">
+      <c r="F29" s="14"/>
+      <c r="G29" s="13">
         <v>2</v>
       </c>
-      <c r="H29" s="12"/>
-      <c r="I29" s="13">
+      <c r="H29" s="14"/>
+      <c r="I29" s="5">
         <v>1.0746999999999999E-30</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="17">
+      <c r="B30" s="7">
         <v>3</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="18">
+      <c r="D30" s="10"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="9">
         <v>6</v>
       </c>
-      <c r="H30" s="19"/>
-      <c r="I30" s="20">
+      <c r="H30" s="10"/>
+      <c r="I30" s="8">
         <v>1.3277E-30</v>
       </c>
     </row>
@@ -1150,94 +1202,80 @@
       <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="14" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="15"/>
-      <c r="G34" s="14" t="s">
+      <c r="F34" s="16"/>
+      <c r="G34" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H34" s="15"/>
-      <c r="I34" s="16" t="s">
+      <c r="H34" s="16"/>
+      <c r="I34" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="4">
+      <c r="B35" s="2">
         <v>1</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5">
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11">
         <v>5</v>
       </c>
-      <c r="H35" s="5"/>
-      <c r="I35" s="6">
+      <c r="H35" s="11"/>
+      <c r="I35" s="3">
         <v>1.0246E-30</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="9">
+      <c r="B36" s="4">
         <v>2</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="11">
+      <c r="D36" s="12"/>
+      <c r="E36" s="13">
         <v>3</v>
       </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="11">
+      <c r="F36" s="14"/>
+      <c r="G36" s="13">
         <v>4</v>
       </c>
-      <c r="H36" s="12"/>
-      <c r="I36" s="13">
+      <c r="H36" s="14"/>
+      <c r="I36" s="5">
         <v>8.9918E-30</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="17">
+      <c r="B37" s="7">
         <v>3</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="18">
+      <c r="D37" s="10"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="9">
         <v>7</v>
       </c>
-      <c r="H37" s="19"/>
-      <c r="I37" s="20">
+      <c r="H37" s="10"/>
+      <c r="I37" s="8">
         <v>1.1055000000000001E-30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="G34:H34"/>
     <mergeCell ref="J15:S18"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="G29:H29"/>
@@ -1252,8 +1290,141 @@
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="G35:H35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4A34E1-7E0A-4996-9F59-C247ACEAA7F9}">
+  <sheetPr>
+    <tabColor theme="6" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="B3:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="22">
+        <v>1</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="25">
+        <v>0.17510000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="23">
+        <v>2</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="26">
+        <v>0.27239999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="24">
+        <v>3</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="27">
+        <v>0.54139999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="22">
+        <v>1</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="25">
+        <v>0.7742</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="23">
+        <v>2</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="26">
+        <v>0.8054</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="24">
+        <v>3</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="27">
+        <v>0.87419999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>